<commit_message>
added detection of end of routine, added ToString() to provide disassembly, added more specificity to opcodes to help static analysis
</commit_message>
<xml_diff>
--- a/ZMachine/data/opcodemeta.xlsx
+++ b/ZMachine/data/opcodemeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\src\zmachine\ZMachine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595FE0B6-A95B-4F27-A61F-BD6C545E07D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD179B51-030D-4075-B8DA-60E670D39856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{990823DD-6830-4DDF-ADA9-D9489FB0AEBD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{990823DD-6830-4DDF-ADA9-D9489FB0AEBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="202">
   <si>
     <t>Opcode</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>Branch</t>
+  </si>
+  <si>
+    <t>return</t>
   </si>
 </sst>
 </file>
@@ -1011,28 +1014,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615CECDA-7B30-49D1-9C77-9020BCF60A7A}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34" style="1"/>
-    <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="17.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="34" style="1"/>
+    <col min="7" max="8" width="34" style="1"/>
+    <col min="9" max="9" width="26.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="17.7265625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="34" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>199</v>
       </c>
@@ -1054,8 +1057,9 @@
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1073,28 +1077,29 @@
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="str">
+      <c r="H2" s="2"/>
+      <c r="I2" s="1" t="str">
         <f>G2 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C2,5,10)),2) &amp; ","</f>
         <v>je=0x01,</v>
       </c>
-      <c r="I2" s="1" t="str">
+      <c r="J2" s="1" t="str">
         <f>IF(A2&lt;&gt;"","Store","")</f>
         <v/>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="K2" s="1" t="str">
         <f>IF(B2&lt;&gt;"","Branch","")</f>
         <v>Branch</v>
       </c>
-      <c r="K2" s="1" t="str">
-        <f t="shared" ref="K2:K33" si="0">IF(AND( A2="", B2=""),"None","")</f>
-        <v/>
-      </c>
       <c r="L2" s="1" t="str">
-        <f>"{ Opcodes." &amp; G2 &amp; ", InstructionSpecialTypes." &amp; I2 &amp; J2 &amp; K2 &amp; "},"</f>
+        <f t="shared" ref="L2:L11" si="0">IF(AND( A2="", B2=""),"None","")</f>
+        <v/>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f t="shared" ref="M2:M33" si="1">"{ Opcodes." &amp; G2 &amp; ", InstructionSpecialTypes." &amp; J2 &amp; K2 &amp; L2 &amp; "},"</f>
         <v>{ Opcodes.je, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -1112,28 +1117,29 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H66" si="1">G3 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C3,5,10)),2) &amp; ","</f>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I66" si="2">G3 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C3,5,10)),2) &amp; ","</f>
         <v>jl=0x02,</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I66" si="2">IF(A3&lt;&gt;"","Store","")</f>
-        <v/>
-      </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J66" si="3">IF(B3&lt;&gt;"","Branch","")</f>
+        <f t="shared" ref="J3:J66" si="3">IF(A3&lt;&gt;"","Store","")</f>
+        <v/>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:K66" si="4">IF(B3&lt;&gt;"","Branch","")</f>
         <v>Branch</v>
       </c>
-      <c r="K3" s="1" t="str">
+      <c r="L3" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L3" s="1" t="str">
-        <f>"{ Opcodes." &amp; G3 &amp; ", InstructionSpecialTypes." &amp; I3 &amp; J3 &amp; K3 &amp; "},"</f>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>{ Opcodes.jl, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -1151,28 +1157,29 @@
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="1" t="str">
+      <c r="H4" s="2"/>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>jg=0x03,</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>jg=0x03,</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L4" s="1" t="str">
-        <f>"{ Opcodes." &amp; G4 &amp; ", InstructionSpecialTypes." &amp; I4 &amp; J4 &amp; K4 &amp; "},"</f>
         <v>{ Opcodes.jg, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1190,28 +1197,29 @@
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="str">
+      <c r="H5" s="2"/>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dec_chk=0x04,</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dec_chk=0x04,</v>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L5" s="1" t="str">
-        <f>"{ Opcodes." &amp; G5 &amp; ", InstructionSpecialTypes." &amp; I5 &amp; J5 &amp; K5 &amp; "},"</f>
         <v>{ Opcodes.dec_chk, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -1229,28 +1237,29 @@
       <c r="G6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="H6" s="2"/>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>inc_chk=0x05,</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>inc_chk=0x05,</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L6" s="1" t="str">
-        <f>"{ Opcodes." &amp; G6 &amp; ", InstructionSpecialTypes." &amp; I6 &amp; J6 &amp; K6 &amp; "},"</f>
         <v>{ Opcodes.inc_chk, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -1268,28 +1277,29 @@
       <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="H7" s="2"/>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>jin=0x06,</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>jin=0x06,</v>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f>"{ Opcodes." &amp; G7 &amp; ", InstructionSpecialTypes." &amp; I7 &amp; J7 &amp; K7 &amp; "},"</f>
         <v>{ Opcodes.jin, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1307,28 +1317,29 @@
       <c r="G8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="H8" s="2"/>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>test=0x07,</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>test=0x07,</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f>"{ Opcodes." &amp; G8 &amp; ", InstructionSpecialTypes." &amp; I8 &amp; J8 &amp; K8 &amp; "},"</f>
         <v>{ Opcodes.test, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1346,28 +1357,29 @@
       <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="H9" s="2"/>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>or=0x08,</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>or=0x08,</v>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L9" s="1" t="str">
-        <f>"{ Opcodes." &amp; G9 &amp; ", InstructionSpecialTypes." &amp; I9 &amp; J9 &amp; K9 &amp; "},"</f>
         <v>{ Opcodes.or, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1385,28 +1397,29 @@
       <c r="G10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="H10" s="2"/>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>and=0x09,</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>and=0x09,</v>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L10" s="1" t="str">
-        <f>"{ Opcodes." &amp; G10 &amp; ", InstructionSpecialTypes." &amp; I10 &amp; J10 &amp; K10 &amp; "},"</f>
         <v>{ Opcodes.and, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1424,28 +1437,29 @@
       <c r="G11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="H11" s="2"/>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>test_attr=0x0A,</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>test_attr=0x0A,</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L11" s="1" t="str">
-        <f>"{ Opcodes." &amp; G11 &amp; ", InstructionSpecialTypes." &amp; I11 &amp; J11 &amp; K11 &amp; "},"</f>
         <v>{ Opcodes.test_attr, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
@@ -1461,28 +1475,29 @@
       <c r="G12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>set_attr=0x0B,</v>
       </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L12" s="1" t="str">
         <f>IF(AND( A12="", B12=""),"None","")</f>
         <v>None</v>
       </c>
-      <c r="L12" s="1" t="str">
-        <f>"{ Opcodes." &amp; G12 &amp; ", InstructionSpecialTypes." &amp; I12 &amp; J12 &amp; K12 &amp; "},"</f>
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>{ Opcodes.set_attr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -1498,28 +1513,29 @@
       <c r="G13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="H13" s="2"/>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>clear_attr=0x0C,</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L13" s="1" t="str">
+        <f t="shared" ref="L13:L66" si="5">IF(AND( A13="", B13=""),"None","")</f>
+        <v>None</v>
+      </c>
+      <c r="M13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>clear_attr=0x0C,</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K13" s="1" t="str">
-        <f t="shared" ref="K13:K66" si="4">IF(AND( A13="", B13=""),"None","")</f>
-        <v>None</v>
-      </c>
-      <c r="L13" s="1" t="str">
-        <f>"{ Opcodes." &amp; G13 &amp; ", InstructionSpecialTypes." &amp; I13 &amp; J13 &amp; K13 &amp; "},"</f>
         <v>{ Opcodes.clear_attr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1535,28 +1551,29 @@
       <c r="G14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="H14" s="2"/>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>store=0x0D,</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>None</v>
+      </c>
+      <c r="M14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>store=0x0D,</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>None</v>
-      </c>
-      <c r="L14" s="1" t="str">
-        <f>"{ Opcodes." &amp; G14 &amp; ", InstructionSpecialTypes." &amp; I14 &amp; J14 &amp; K14 &amp; "},"</f>
         <v>{ Opcodes.store, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -1572,28 +1589,29 @@
       <c r="G15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="H15" s="2"/>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>insert_obj=0x0E,</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L15" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>None</v>
+      </c>
+      <c r="M15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert_obj=0x0E,</v>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>None</v>
-      </c>
-      <c r="L15" s="1" t="str">
-        <f>"{ Opcodes." &amp; G15 &amp; ", InstructionSpecialTypes." &amp; I15 &amp; J15 &amp; K15 &amp; "},"</f>
         <v>{ Opcodes.insert_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1611,28 +1629,29 @@
       <c r="G16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="H16" s="2"/>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>loadw=0x0F,</v>
+      </c>
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>loadw=0x0F,</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L16" s="1" t="str">
-        <f>"{ Opcodes." &amp; G16 &amp; ", InstructionSpecialTypes." &amp; I16 &amp; J16 &amp; K16 &amp; "},"</f>
         <v>{ Opcodes.loadw, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1650,28 +1669,29 @@
       <c r="G17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="H17" s="2"/>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>loadb=0x10,</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>loadb=0x10,</v>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L17" s="1" t="str">
-        <f>"{ Opcodes." &amp; G17 &amp; ", InstructionSpecialTypes." &amp; I17 &amp; J17 &amp; K17 &amp; "},"</f>
         <v>{ Opcodes.loadb, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1689,28 +1709,29 @@
       <c r="G18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="1" t="str">
+      <c r="H18" s="2"/>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_prop=0x11,</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L18" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_prop=0x11,</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K18" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L18" s="1" t="str">
-        <f>"{ Opcodes." &amp; G18 &amp; ", InstructionSpecialTypes." &amp; I18 &amp; J18 &amp; K18 &amp; "},"</f>
         <v>{ Opcodes.get_prop, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -1728,28 +1749,29 @@
       <c r="G19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="1" t="str">
+      <c r="H19" s="2"/>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_prop_addr=0x12,</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L19" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_prop_addr=0x12,</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K19" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L19" s="1" t="str">
-        <f>"{ Opcodes." &amp; G19 &amp; ", InstructionSpecialTypes." &amp; I19 &amp; J19 &amp; K19 &amp; "},"</f>
         <v>{ Opcodes.get_prop_addr, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1767,28 +1789,29 @@
       <c r="G20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="1" t="str">
+      <c r="H20" s="2"/>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_next_prop=0x13,</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L20" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_next_prop=0x13,</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L20" s="1" t="str">
-        <f>"{ Opcodes." &amp; G20 &amp; ", InstructionSpecialTypes." &amp; I20 &amp; J20 &amp; K20 &amp; "},"</f>
         <v>{ Opcodes.get_next_prop, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1806,28 +1829,29 @@
       <c r="G21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H21" s="1" t="str">
+      <c r="H21" s="2"/>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>add=0x14,</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L21" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>add=0x14,</v>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L21" s="1" t="str">
-        <f>"{ Opcodes." &amp; G21 &amp; ", InstructionSpecialTypes." &amp; I21 &amp; J21 &amp; K21 &amp; "},"</f>
         <v>{ Opcodes.add, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1845,28 +1869,29 @@
       <c r="G22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="1" t="str">
+      <c r="H22" s="2"/>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>sub=0x15,</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L22" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>sub=0x15,</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K22" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L22" s="1" t="str">
-        <f>"{ Opcodes." &amp; G22 &amp; ", InstructionSpecialTypes." &amp; I22 &amp; J22 &amp; K22 &amp; "},"</f>
         <v>{ Opcodes.sub, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1884,28 +1909,29 @@
       <c r="G23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="1" t="str">
+      <c r="H23" s="2"/>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>mul=0x16,</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L23" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>mul=0x16,</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L23" s="1" t="str">
-        <f>"{ Opcodes." &amp; G23 &amp; ", InstructionSpecialTypes." &amp; I23 &amp; J23 &amp; K23 &amp; "},"</f>
         <v>{ Opcodes.mul, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1923,28 +1949,29 @@
       <c r="G24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="1" t="str">
+      <c r="H24" s="2"/>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>div=0x17,</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L24" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>div=0x17,</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K24" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L24" s="1" t="str">
-        <f>"{ Opcodes." &amp; G24 &amp; ", InstructionSpecialTypes." &amp; I24 &amp; J24 &amp; K24 &amp; "},"</f>
         <v>{ Opcodes.div, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -1962,28 +1989,29 @@
       <c r="G25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="H25" s="2"/>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>mod=0x18,</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L25" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>mod=0x18,</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K25" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L25" s="1" t="str">
-        <f>"{ Opcodes." &amp; G25 &amp; ", InstructionSpecialTypes." &amp; I25 &amp; J25 &amp; K25 &amp; "},"</f>
         <v>{ Opcodes.mod, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -2001,28 +2029,29 @@
       <c r="G26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="1" t="str">
+      <c r="H26" s="2"/>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>jz=0x80,</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>jz=0x80,</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K26" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L26" s="1" t="str">
-        <f>"{ Opcodes." &amp; G26 &amp; ", InstructionSpecialTypes." &amp; I26 &amp; J26 &amp; K26 &amp; "},"</f>
         <v>{ Opcodes.jz, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
@@ -2042,28 +2071,29 @@
       <c r="G27" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H27" s="1" t="str">
+      <c r="H27" s="2"/>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_sibling=0x81,</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L27" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_sibling=0x81,</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K27" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L27" s="1" t="str">
-        <f>"{ Opcodes." &amp; G27 &amp; ", InstructionSpecialTypes." &amp; I27 &amp; J27 &amp; K27 &amp; "},"</f>
         <v>{ Opcodes.get_sibling, InstructionSpecialTypes.StoreBranch},</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
@@ -2083,28 +2113,29 @@
       <c r="G28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H28" s="1" t="str">
+      <c r="H28" s="2"/>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_child=0x82,</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Branch</v>
+      </c>
+      <c r="L28" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_child=0x82,</v>
-      </c>
-      <c r="I28" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>Branch</v>
-      </c>
-      <c r="K28" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L28" s="1" t="str">
-        <f>"{ Opcodes." &amp; G28 &amp; ", InstructionSpecialTypes." &amp; I28 &amp; J28 &amp; K28 &amp; "},"</f>
         <v>{ Opcodes.get_child, InstructionSpecialTypes.StoreBranch},</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
@@ -2122,28 +2153,29 @@
       <c r="G29" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H29" s="1" t="str">
+      <c r="H29" s="2"/>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_parent=0x83,</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L29" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_parent=0x83,</v>
-      </c>
-      <c r="I29" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L29" s="1" t="str">
-        <f>"{ Opcodes." &amp; G29 &amp; ", InstructionSpecialTypes." &amp; I29 &amp; J29 &amp; K29 &amp; "},"</f>
         <v>{ Opcodes.get_parent, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
@@ -2161,28 +2193,29 @@
       <c r="G30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H30" s="1" t="str">
+      <c r="H30" s="2"/>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>get_prop_len=0x84,</v>
+      </c>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Store</v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L30" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>get_prop_len=0x84,</v>
-      </c>
-      <c r="I30" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Store</v>
-      </c>
-      <c r="J30" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K30" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="L30" s="1" t="str">
-        <f>"{ Opcodes." &amp; G30 &amp; ", InstructionSpecialTypes." &amp; I30 &amp; J30 &amp; K30 &amp; "},"</f>
         <v>{ Opcodes.get_prop_len, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
@@ -2198,28 +2231,29 @@
       <c r="G31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H31" s="1" t="str">
+      <c r="H31" s="2"/>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>inc=0x85,</v>
+      </c>
+      <c r="J31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L31" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>None</v>
+      </c>
+      <c r="M31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>inc=0x85,</v>
-      </c>
-      <c r="I31" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J31" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K31" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>None</v>
-      </c>
-      <c r="L31" s="1" t="str">
-        <f>"{ Opcodes." &amp; G31 &amp; ", InstructionSpecialTypes." &amp; I31 &amp; J31 &amp; K31 &amp; "},"</f>
         <v>{ Opcodes.inc, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
@@ -2235,28 +2269,29 @@
       <c r="G32" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H32" s="1" t="str">
+      <c r="H32" s="2"/>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dec=0x86,</v>
+      </c>
+      <c r="J32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L32" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>None</v>
+      </c>
+      <c r="M32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dec=0x86,</v>
-      </c>
-      <c r="I32" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J32" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K32" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>None</v>
-      </c>
-      <c r="L32" s="1" t="str">
-        <f>"{ Opcodes." &amp; G32 &amp; ", InstructionSpecialTypes." &amp; I32 &amp; J32 &amp; K32 &amp; "},"</f>
         <v>{ Opcodes.dec, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
@@ -2272,28 +2307,29 @@
       <c r="G33" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H33" s="1" t="str">
+      <c r="H33" s="2"/>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>print_addr=0x87,</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L33" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>None</v>
+      </c>
+      <c r="M33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>print_addr=0x87,</v>
-      </c>
-      <c r="I33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J33" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K33" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>None</v>
-      </c>
-      <c r="L33" s="1" t="str">
-        <f>"{ Opcodes." &amp; G33 &amp; ", InstructionSpecialTypes." &amp; I33 &amp; J33 &amp; K33 &amp; "},"</f>
         <v>{ Opcodes.print_addr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -2309,28 +2345,29 @@
       <c r="G34" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H34" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>remove_obj=0x89,</v>
       </c>
-      <c r="I34" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J34" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K34" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L34" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L34" s="1" t="str">
-        <f>"{ Opcodes." &amp; G34 &amp; ", InstructionSpecialTypes." &amp; I34 &amp; J34 &amp; K34 &amp; "},"</f>
+      <c r="M34" s="1" t="str">
+        <f t="shared" ref="M34:M65" si="6">"{ Opcodes." &amp; G34 &amp; ", InstructionSpecialTypes." &amp; J34 &amp; K34 &amp; L34 &amp; "},"</f>
         <v>{ Opcodes.remove_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
@@ -2346,28 +2383,29 @@
       <c r="G35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H35" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print_obj=0x8A,</v>
       </c>
-      <c r="I35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J35" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K35" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L35" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L35" s="1" t="str">
-        <f>"{ Opcodes." &amp; G35 &amp; ", InstructionSpecialTypes." &amp; I35 &amp; J35 &amp; K35 &amp; "},"</f>
+      <c r="M35" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
@@ -2383,28 +2421,31 @@
       <c r="G36" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>ret=0x8B,</v>
       </c>
-      <c r="I36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J36" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K36" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L36" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L36" s="1" t="str">
-        <f>"{ Opcodes." &amp; G36 &amp; ", InstructionSpecialTypes." &amp; I36 &amp; J36 &amp; K36 &amp; "},"</f>
+      <c r="M36" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.ret, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
@@ -2420,28 +2461,29 @@
       <c r="G37" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H37" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>jump=0x8C,</v>
       </c>
-      <c r="I37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J37" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K37" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L37" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L37" s="1" t="str">
-        <f>"{ Opcodes." &amp; G37 &amp; ", InstructionSpecialTypes." &amp; I37 &amp; J37 &amp; K37 &amp; "},"</f>
+      <c r="M37" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.jump, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -2457,28 +2499,29 @@
       <c r="G38" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print_paddr=0x8D,</v>
       </c>
-      <c r="I38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J38" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K38" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L38" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L38" s="1" t="str">
-        <f>"{ Opcodes." &amp; G38 &amp; ", InstructionSpecialTypes." &amp; I38 &amp; J38 &amp; K38 &amp; "},"</f>
+      <c r="M38" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print_paddr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>5</v>
       </c>
@@ -2496,28 +2539,29 @@
       <c r="G39" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H39" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>load=0x8E,</v>
       </c>
-      <c r="I39" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="J39" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Store</v>
       </c>
-      <c r="J39" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="K39" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L39" s="1" t="str">
-        <f>"{ Opcodes." &amp; G39 &amp; ", InstructionSpecialTypes." &amp; I39 &amp; J39 &amp; K39 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M39" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.load, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
@@ -2533,28 +2577,31 @@
       <c r="G40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H40" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H40" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>rtrue=0xB0,</v>
       </c>
-      <c r="I40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J40" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K40" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L40" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L40" s="1" t="str">
-        <f>"{ Opcodes." &amp; G40 &amp; ", InstructionSpecialTypes." &amp; I40 &amp; J40 &amp; K40 &amp; "},"</f>
+      <c r="M40" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.rtrue, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
@@ -2570,28 +2617,31 @@
       <c r="G41" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H41" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H41" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>rfalse=0xB1,</v>
       </c>
-      <c r="I41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J41" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K41" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L41" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L41" s="1" t="str">
-        <f>"{ Opcodes." &amp; G41 &amp; ", InstructionSpecialTypes." &amp; I41 &amp; J41 &amp; K41 &amp; "},"</f>
+      <c r="M41" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.rfalse, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -2607,28 +2657,29 @@
       <c r="G42" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H42" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print=0xB2,</v>
       </c>
-      <c r="I42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J42" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K42" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L42" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L42" s="1" t="str">
-        <f>"{ Opcodes." &amp; G42 &amp; ", InstructionSpecialTypes." &amp; I42 &amp; J42 &amp; K42 &amp; "},"</f>
+      <c r="M42" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
@@ -2644,28 +2695,31 @@
       <c r="G43" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H43" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print_ret=0xB3,</v>
       </c>
-      <c r="I43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J43" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K43" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L43" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L43" s="1" t="str">
-        <f>"{ Opcodes." &amp; G43 &amp; ", InstructionSpecialTypes." &amp; I43 &amp; J43 &amp; K43 &amp; "},"</f>
+      <c r="M43" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print_ret, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2685,28 +2739,29 @@
       <c r="G44" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H44" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>save=0xB5,</v>
       </c>
-      <c r="I44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J44" s="1" t="str">
         <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Branch</v>
       </c>
-      <c r="K44" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L44" s="1" t="str">
-        <f>"{ Opcodes." &amp; G44 &amp; ", InstructionSpecialTypes." &amp; I44 &amp; J44 &amp; K44 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M44" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.save, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2726,28 +2781,29 @@
       <c r="G45" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H45" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>restore=0xB6,</v>
       </c>
-      <c r="I45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J45" s="1" t="str">
         <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K45" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Branch</v>
       </c>
-      <c r="K45" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L45" s="1" t="str">
-        <f>"{ Opcodes." &amp; G45 &amp; ", InstructionSpecialTypes." &amp; I45 &amp; J45 &amp; K45 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M45" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.restore, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -2763,28 +2819,29 @@
       <c r="G46" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H46" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>restart=0xB7,</v>
       </c>
-      <c r="I46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J46" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K46" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L46" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L46" s="1" t="str">
-        <f>"{ Opcodes." &amp; G46 &amp; ", InstructionSpecialTypes." &amp; I46 &amp; J46 &amp; K46 &amp; "},"</f>
+      <c r="M46" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.restart, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
@@ -2800,28 +2857,31 @@
       <c r="G47" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H47" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H47" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>ret_popped=0xB8,</v>
       </c>
-      <c r="I47" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J47" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K47" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L47" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L47" s="1" t="str">
-        <f>"{ Opcodes." &amp; G47 &amp; ", InstructionSpecialTypes." &amp; I47 &amp; J47 &amp; K47 &amp; "},"</f>
+      <c r="M47" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.ret_popped, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
@@ -2839,28 +2899,29 @@
       <c r="G48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H48" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>pop=0xB9,</v>
       </c>
-      <c r="I48" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J48" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K48" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L48" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L48" s="1" t="str">
-        <f>"{ Opcodes." &amp; G48 &amp; ", InstructionSpecialTypes." &amp; I48 &amp; J48 &amp; K48 &amp; "},"</f>
+      <c r="M48" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.pop, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
@@ -2876,28 +2937,31 @@
       <c r="G49" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H49" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H49" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>quit=0xBA,</v>
       </c>
-      <c r="I49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J49" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K49" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L49" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L49" s="1" t="str">
-        <f>"{ Opcodes." &amp; G49 &amp; ", InstructionSpecialTypes." &amp; I49 &amp; J49 &amp; K49 &amp; "},"</f>
+      <c r="M49" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.quit, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
@@ -2913,28 +2977,29 @@
       <c r="G50" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H50" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>new_line=0xBB,</v>
       </c>
-      <c r="I50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J50" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K50" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L50" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L50" s="1" t="str">
-        <f>"{ Opcodes." &amp; G50 &amp; ", InstructionSpecialTypes." &amp; I50 &amp; J50 &amp; K50 &amp; "},"</f>
+      <c r="M50" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.new_line, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
@@ -2952,28 +3017,29 @@
       <c r="G51" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H51" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>show_status=0xBC,</v>
       </c>
-      <c r="I51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J51" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K51" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L51" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L51" s="1" t="str">
-        <f>"{ Opcodes." &amp; G51 &amp; ", InstructionSpecialTypes." &amp; I51 &amp; J51 &amp; K51 &amp; "},"</f>
+      <c r="M51" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.show_status, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2993,28 +3059,29 @@
       <c r="G52" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H52" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>verify=0xBD,</v>
       </c>
-      <c r="I52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J52" s="1" t="str">
         <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K52" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Branch</v>
       </c>
-      <c r="K52" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L52" s="1" t="str">
-        <f>"{ Opcodes." &amp; G52 &amp; ", InstructionSpecialTypes." &amp; I52 &amp; J52 &amp; K52 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M52" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.verify, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>5</v>
       </c>
@@ -3034,28 +3101,29 @@
       <c r="G53" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H53" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>call=0xE0,</v>
       </c>
-      <c r="I53" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="J53" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Store</v>
       </c>
-      <c r="J53" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="K53" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L53" s="1" t="str">
-        <f>"{ Opcodes." &amp; G53 &amp; ", InstructionSpecialTypes." &amp; I53 &amp; J53 &amp; K53 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M53" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.call, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
@@ -3071,28 +3139,29 @@
       <c r="G54" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>storew=0xE1,</v>
       </c>
-      <c r="I54" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J54" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K54" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L54" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L54" s="1" t="str">
-        <f>"{ Opcodes." &amp; G54 &amp; ", InstructionSpecialTypes." &amp; I54 &amp; J54 &amp; K54 &amp; "},"</f>
+      <c r="M54" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.storew, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
@@ -3108,28 +3177,29 @@
       <c r="G55" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="H55" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>storeb=0xE2,</v>
       </c>
-      <c r="I55" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J55" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K55" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L55" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L55" s="1" t="str">
-        <f>"{ Opcodes." &amp; G55 &amp; ", InstructionSpecialTypes." &amp; I55 &amp; J55 &amp; K55 &amp; "},"</f>
+      <c r="M55" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.storeb, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
@@ -3145,28 +3215,29 @@
       <c r="G56" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H56" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>put_prop=0xE3,</v>
       </c>
-      <c r="I56" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J56" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K56" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L56" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L56" s="1" t="str">
-        <f>"{ Opcodes." &amp; G56 &amp; ", InstructionSpecialTypes." &amp; I56 &amp; J56 &amp; K56 &amp; "},"</f>
+      <c r="M56" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.put_prop, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
@@ -3184,28 +3255,29 @@
       <c r="G57" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H57" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>sread=0xE4,</v>
       </c>
-      <c r="I57" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J57" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K57" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L57" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L57" s="1" t="str">
-        <f>"{ Opcodes." &amp; G57 &amp; ", InstructionSpecialTypes." &amp; I57 &amp; J57 &amp; K57 &amp; "},"</f>
+      <c r="M57" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.sread, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
@@ -3221,28 +3293,29 @@
       <c r="G58" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H58" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print_char=0xE5,</v>
       </c>
-      <c r="I58" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J58" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K58" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L58" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L58" s="1" t="str">
-        <f>"{ Opcodes." &amp; G58 &amp; ", InstructionSpecialTypes." &amp; I58 &amp; J58 &amp; K58 &amp; "},"</f>
+      <c r="M58" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print_char, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
@@ -3258,28 +3331,29 @@
       <c r="G59" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H59" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>print_num=0xE6,</v>
       </c>
-      <c r="I59" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J59" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K59" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L59" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L59" s="1" t="str">
-        <f>"{ Opcodes." &amp; G59 &amp; ", InstructionSpecialTypes." &amp; I59 &amp; J59 &amp; K59 &amp; "},"</f>
+      <c r="M59" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.print_num, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
@@ -3297,28 +3371,29 @@
       <c r="G60" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H60" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>random=0xE7,</v>
       </c>
-      <c r="I60" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="J60" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Store</v>
       </c>
-      <c r="J60" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="K60" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L60" s="1" t="str">
-        <f>"{ Opcodes." &amp; G60 &amp; ", InstructionSpecialTypes." &amp; I60 &amp; J60 &amp; K60 &amp; "},"</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M60" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.random, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
@@ -3334,28 +3409,29 @@
       <c r="G61" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H61" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>push=0xE8,</v>
       </c>
-      <c r="I61" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J61" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K61" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L61" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L61" s="1" t="str">
-        <f>"{ Opcodes." &amp; G61 &amp; ", InstructionSpecialTypes." &amp; I61 &amp; J61 &amp; K61 &amp; "},"</f>
+      <c r="M61" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.push, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
@@ -3373,28 +3449,29 @@
       <c r="G62" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H62" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>pull=0xE9,</v>
       </c>
-      <c r="I62" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J62" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K62" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L62" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L62" s="1" t="str">
-        <f>"{ Opcodes." &amp; G62 &amp; ", InstructionSpecialTypes." &amp; I62 &amp; J62 &amp; K62 &amp; "},"</f>
+      <c r="M62" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.pull, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
@@ -3412,28 +3489,29 @@
       <c r="G63" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="H63" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>split_window=0xEA,</v>
       </c>
-      <c r="I63" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J63" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K63" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L63" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L63" s="1" t="str">
-        <f>"{ Opcodes." &amp; G63 &amp; ", InstructionSpecialTypes." &amp; I63 &amp; J63 &amp; K63 &amp; "},"</f>
+      <c r="M63" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.split_window, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
@@ -3451,28 +3529,29 @@
       <c r="G64" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H64" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>set_window=0xEB,</v>
       </c>
-      <c r="I64" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J64" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K64" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L64" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L64" s="1" t="str">
-        <f>"{ Opcodes." &amp; G64 &amp; ", InstructionSpecialTypes." &amp; I64 &amp; J64 &amp; K64 &amp; "},"</f>
+      <c r="M64" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.set_window, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
@@ -3490,28 +3569,29 @@
       <c r="G65" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="H65" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>output_stream=0xF3,</v>
       </c>
-      <c r="I65" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J65" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K65" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L65" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L65" s="1" t="str">
-        <f>"{ Opcodes." &amp; G65 &amp; ", InstructionSpecialTypes." &amp; I65 &amp; J65 &amp; K65 &amp; "},"</f>
+      <c r="M65" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>{ Opcodes.output_stream, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
@@ -3529,24 +3609,25 @@
       <c r="G66" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H66" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>input_stream=0xF4,</v>
       </c>
-      <c r="I66" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="J66" s="1" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K66" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L66" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>None</v>
       </c>
-      <c r="L66" s="1" t="str">
-        <f>"{ Opcodes." &amp; G66 &amp; ", InstructionSpecialTypes." &amp; I66 &amp; J66 &amp; K66 &amp; "},"</f>
+      <c r="M66" s="1" t="str">
+        <f t="shared" ref="M66:M97" si="7">"{ Opcodes." &amp; G66 &amp; ", InstructionSpecialTypes." &amp; J66 &amp; K66 &amp; L66 &amp; "},"</f>
         <v>{ Opcodes.input_stream, InstructionSpecialTypes.None},</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed opcode values in enums to avoid issues, started text decode
</commit_message>
<xml_diff>
--- a/ZMachine/data/opcodemeta.xlsx
+++ b/ZMachine/data/opcodemeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\src\zmachine\ZMachine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD179B51-030D-4075-B8DA-60E670D39856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0CF99-87ED-45CE-A5F0-8B2877E25629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{990823DD-6830-4DDF-ADA9-D9489FB0AEBD}"/>
   </bookViews>
@@ -1014,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615CECDA-7B30-49D1-9C77-9020BCF60A7A}">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I66" sqref="I2:I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1028,14 +1028,14 @@
     <col min="4" max="4" width="4.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="8" width="34" style="1"/>
-    <col min="9" max="9" width="26.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="17.7265625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="34" style="1"/>
+    <col min="7" max="9" width="34" style="1"/>
+    <col min="10" max="10" width="26.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="17.7265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="34" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>199</v>
       </c>
@@ -1058,8 +1058,9 @@
         <v>4</v>
       </c>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1078,28 +1079,32 @@
         <v>8</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="1" t="str">
+      <c r="I2" s="2" t="str">
+        <f>G2 &amp;"=0x" &amp; RIGHT("0" &amp;  DEC2HEX( MID(C2,5,10)),2) &amp; ","</f>
+        <v>je=0x01,</v>
+      </c>
+      <c r="J2" s="1" t="str">
         <f>G2 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C2,5,10)),2) &amp; ","</f>
         <v>je=0x01,</v>
       </c>
-      <c r="J2" s="1" t="str">
+      <c r="K2" s="1" t="str">
         <f>IF(A2&lt;&gt;"","Store","")</f>
         <v/>
       </c>
-      <c r="K2" s="1" t="str">
+      <c r="L2" s="1" t="str">
         <f>IF(B2&lt;&gt;"","Branch","")</f>
         <v>Branch</v>
       </c>
-      <c r="L2" s="1" t="str">
-        <f t="shared" ref="L2:L11" si="0">IF(AND( A2="", B2=""),"None","")</f>
-        <v/>
-      </c>
       <c r="M2" s="1" t="str">
-        <f t="shared" ref="M2:M33" si="1">"{ Opcodes." &amp; G2 &amp; ", InstructionSpecialTypes." &amp; J2 &amp; K2 &amp; L2 &amp; "},"</f>
+        <f t="shared" ref="M2:M11" si="0">IF(AND( A2="", B2=""),"None","")</f>
+        <v/>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f t="shared" ref="N2:N33" si="1">"{ Opcodes." &amp; G2 &amp; ", InstructionSpecialTypes." &amp; K2 &amp; L2 &amp; M2 &amp; "},"</f>
         <v>{ Opcodes.je, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -1118,28 +1123,32 @@
         <v>11</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I66" si="2">G3 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C3,5,10)),2) &amp; ","</f>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I66" si="2">G3 &amp;"=0x" &amp; RIGHT("0" &amp;  DEC2HEX( MID(C3,5,10)),2) &amp; ","</f>
         <v>jl=0x02,</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J66" si="3">IF(A3&lt;&gt;"","Store","")</f>
-        <v/>
+        <f t="shared" ref="J3:J66" si="3">G3 &amp; "=0x" &amp;  RIGHT("00" &amp; DEC2HEX(MID(C3,5,10)),2) &amp; ","</f>
+        <v>jl=0x02,</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f t="shared" ref="K3:K66" si="4">IF(B3&lt;&gt;"","Branch","")</f>
+        <f t="shared" ref="K3:K66" si="4">IF(A3&lt;&gt;"","Store","")</f>
+        <v/>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f t="shared" ref="L3:L66" si="5">IF(B3&lt;&gt;"","Branch","")</f>
         <v>Branch</v>
       </c>
-      <c r="L3" s="1" t="str">
+      <c r="M3" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M3" s="1" t="str">
+      <c r="N3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.jl, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -1158,28 +1167,32 @@
         <v>14</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="1" t="str">
+      <c r="I4" s="2" t="str">
         <f t="shared" si="2"/>
         <v>jg=0x03,</v>
       </c>
       <c r="J4" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>jg=0x03,</v>
       </c>
       <c r="K4" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L4" s="1" t="str">
+      <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M4" s="1" t="str">
+      <c r="N4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.jg, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1198,28 +1211,32 @@
         <v>17</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="1" t="str">
+      <c r="I5" s="2" t="str">
         <f t="shared" si="2"/>
         <v>dec_chk=0x04,</v>
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>dec_chk=0x04,</v>
       </c>
       <c r="K5" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L5" s="1" t="str">
+      <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M5" s="1" t="str">
+      <c r="N5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.dec_chk, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -1238,28 +1255,32 @@
         <v>20</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="1" t="str">
+      <c r="I6" s="2" t="str">
         <f t="shared" si="2"/>
         <v>inc_chk=0x05,</v>
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>inc_chk=0x05,</v>
       </c>
       <c r="K6" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L6" s="1" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M6" s="1" t="str">
+      <c r="N6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.inc_chk, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -1278,28 +1299,32 @@
         <v>23</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="1" t="str">
+      <c r="I7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>jin=0x06,</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>jin=0x06,</v>
       </c>
       <c r="K7" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L7" s="1" t="str">
+      <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M7" s="1" t="str">
+      <c r="N7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.jin, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -1318,28 +1343,32 @@
         <v>26</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="1" t="str">
+      <c r="I8" s="2" t="str">
         <f t="shared" si="2"/>
         <v>test=0x07,</v>
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>test=0x07,</v>
       </c>
       <c r="K8" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M8" s="1" t="str">
+      <c r="N8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.test, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1358,28 +1387,32 @@
         <v>29</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="1" t="str">
+      <c r="I9" s="2" t="str">
         <f t="shared" si="2"/>
         <v>or=0x08,</v>
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>or=0x08,</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L9" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M9" s="1" t="str">
+      <c r="N9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.or, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1398,28 +1431,32 @@
         <v>32</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="1" t="str">
+      <c r="I10" s="2" t="str">
         <f t="shared" si="2"/>
         <v>and=0x09,</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>and=0x09,</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L10" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M10" s="1" t="str">
+      <c r="N10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.and, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1438,28 +1475,32 @@
         <v>36</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="1" t="str">
+      <c r="I11" s="2" t="str">
         <f t="shared" si="2"/>
         <v>test_attr=0x0A,</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>test_attr=0x0A,</v>
       </c>
       <c r="K11" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L11" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L11" s="1" t="str">
+      <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M11" s="1" t="str">
+      <c r="N11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.test_attr, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
@@ -1476,28 +1517,32 @@
         <v>40</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="1" t="str">
+      <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>set_attr=0x0B,</v>
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>set_attr=0x0B,</v>
       </c>
       <c r="K12" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M12" s="1" t="str">
         <f>IF(AND( A12="", B12=""),"None","")</f>
         <v>None</v>
       </c>
-      <c r="M12" s="1" t="str">
+      <c r="N12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.set_attr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
@@ -1514,28 +1559,32 @@
         <v>44</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="1" t="str">
+      <c r="I13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>clear_attr=0x0C,</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>clear_attr=0x0C,</v>
       </c>
       <c r="K13" s="1" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" ref="L13:L66" si="5">IF(AND( A13="", B13=""),"None","")</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f t="shared" ref="M13:M66" si="6">IF(AND( A13="", B13=""),"None","")</f>
         <v>None</v>
       </c>
-      <c r="M13" s="1" t="str">
+      <c r="N13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.clear_attr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -1552,13 +1601,13 @@
         <v>48</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="1" t="str">
+      <c r="I14" s="2" t="str">
         <f t="shared" si="2"/>
         <v>store=0x0D,</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>store=0x0D,</v>
       </c>
       <c r="K14" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1566,14 +1615,18 @@
       </c>
       <c r="L14" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M14" s="1" t="str">
+      <c r="N14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.store, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
@@ -1590,13 +1643,13 @@
         <v>52</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="1" t="str">
+      <c r="I15" s="2" t="str">
         <f t="shared" si="2"/>
         <v>insert_obj=0x0E,</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>insert_obj=0x0E,</v>
       </c>
       <c r="K15" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1604,14 +1657,18 @@
       </c>
       <c r="L15" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M15" s="1" t="str">
+      <c r="N15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.insert_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1630,28 +1687,32 @@
         <v>56</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="1" t="str">
+      <c r="I16" s="2" t="str">
         <f t="shared" si="2"/>
         <v>loadw=0x0F,</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>loadw=0x0F,</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.loadw, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1670,28 +1731,32 @@
         <v>59</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="1" t="str">
+      <c r="I17" s="2" t="str">
         <f t="shared" si="2"/>
         <v>loadb=0x10,</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>loadb=0x10,</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.loadb, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1710,28 +1775,32 @@
         <v>62</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="1" t="str">
+      <c r="I18" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_prop=0x11,</v>
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_prop=0x11,</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K18" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L18" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_prop, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -1750,28 +1819,32 @@
         <v>65</v>
       </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="1" t="str">
+      <c r="I19" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_prop_addr=0x12,</v>
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_prop_addr=0x12,</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K19" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_prop_addr, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1790,28 +1863,32 @@
         <v>68</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="1" t="str">
+      <c r="I20" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_next_prop=0x13,</v>
       </c>
       <c r="J20" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_next_prop=0x13,</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L20" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M20" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_next_prop, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1830,28 +1907,32 @@
         <v>71</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="1" t="str">
+      <c r="I21" s="2" t="str">
         <f t="shared" si="2"/>
         <v>add=0x14,</v>
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>add=0x14,</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L21" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M21" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.add, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1870,28 +1951,32 @@
         <v>74</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="1" t="str">
+      <c r="I22" s="2" t="str">
         <f t="shared" si="2"/>
         <v>sub=0x15,</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>sub=0x15,</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K22" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L22" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.sub, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1910,28 +1995,32 @@
         <v>77</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="1" t="str">
+      <c r="I23" s="2" t="str">
         <f t="shared" si="2"/>
         <v>mul=0x16,</v>
       </c>
       <c r="J23" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>mul=0x16,</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L23" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.mul, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1950,28 +2039,32 @@
         <v>80</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="1" t="str">
+      <c r="I24" s="2" t="str">
         <f t="shared" si="2"/>
         <v>div=0x17,</v>
       </c>
       <c r="J24" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>div=0x17,</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K24" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L24" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M24" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.div, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -1990,28 +2083,32 @@
         <v>83</v>
       </c>
       <c r="H25" s="2"/>
-      <c r="I25" s="1" t="str">
+      <c r="I25" s="2" t="str">
         <f t="shared" si="2"/>
         <v>mod=0x18,</v>
       </c>
       <c r="J25" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>mod=0x18,</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K25" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L25" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M25" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.mod, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -2030,28 +2127,32 @@
         <v>86</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="1" t="str">
+      <c r="I26" s="2" t="str">
         <f t="shared" si="2"/>
         <v>jz=0x80,</v>
       </c>
       <c r="J26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>jz=0x80,</v>
       </c>
       <c r="K26" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L26" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L26" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M26" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N26" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.jz, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
@@ -2072,28 +2173,32 @@
         <v>89</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="1" t="str">
+      <c r="I27" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_sibling=0x81,</v>
       </c>
       <c r="J27" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_sibling=0x81,</v>
+      </c>
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K27" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="L27" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L27" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M27" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_sibling, InstructionSpecialTypes.StoreBranch},</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
@@ -2114,28 +2219,32 @@
         <v>92</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="1" t="str">
+      <c r="I28" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_child=0x82,</v>
       </c>
       <c r="J28" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_child=0x82,</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K28" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="L28" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L28" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M28" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N28" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_child, InstructionSpecialTypes.StoreBranch},</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
@@ -2154,28 +2263,32 @@
         <v>95</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="1" t="str">
+      <c r="I29" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_parent=0x83,</v>
       </c>
       <c r="J29" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_parent=0x83,</v>
+      </c>
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L29" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M29" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_parent, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
@@ -2194,28 +2307,32 @@
         <v>98</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="1" t="str">
+      <c r="I30" s="2" t="str">
         <f t="shared" si="2"/>
         <v>get_prop_len=0x84,</v>
       </c>
       <c r="J30" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>get_prop_len=0x84,</v>
+      </c>
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K30" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L30" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M30" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N30" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.get_prop_len, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
@@ -2232,13 +2349,13 @@
         <v>101</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="1" t="str">
+      <c r="I31" s="2" t="str">
         <f t="shared" si="2"/>
         <v>inc=0x85,</v>
       </c>
       <c r="J31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>inc=0x85,</v>
       </c>
       <c r="K31" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2246,14 +2363,18 @@
       </c>
       <c r="L31" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M31" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M31" s="1" t="str">
+      <c r="N31" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.inc, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
@@ -2270,13 +2391,13 @@
         <v>104</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="1" t="str">
+      <c r="I32" s="2" t="str">
         <f t="shared" si="2"/>
         <v>dec=0x86,</v>
       </c>
       <c r="J32" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>dec=0x86,</v>
       </c>
       <c r="K32" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2284,14 +2405,18 @@
       </c>
       <c r="L32" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M32" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M32" s="1" t="str">
+      <c r="N32" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.dec, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
@@ -2308,13 +2433,13 @@
         <v>107</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="1" t="str">
+      <c r="I33" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_addr=0x87,</v>
       </c>
       <c r="J33" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_addr=0x87,</v>
       </c>
       <c r="K33" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2322,14 +2447,18 @@
       </c>
       <c r="L33" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M33" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M33" s="1" t="str">
+      <c r="N33" s="1" t="str">
         <f t="shared" si="1"/>
         <v>{ Opcodes.print_addr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
@@ -2346,13 +2475,13 @@
         <v>110</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="1" t="str">
+      <c r="I34" s="2" t="str">
         <f t="shared" si="2"/>
         <v>remove_obj=0x89,</v>
       </c>
       <c r="J34" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>remove_obj=0x89,</v>
       </c>
       <c r="K34" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2360,14 +2489,18 @@
       </c>
       <c r="L34" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M34" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M34" s="1" t="str">
-        <f t="shared" ref="M34:M65" si="6">"{ Opcodes." &amp; G34 &amp; ", InstructionSpecialTypes." &amp; J34 &amp; K34 &amp; L34 &amp; "},"</f>
+      <c r="N34" s="1" t="str">
+        <f t="shared" ref="N34:N65" si="7">"{ Opcodes." &amp; G34 &amp; ", InstructionSpecialTypes." &amp; K34 &amp; L34 &amp; M34 &amp; "},"</f>
         <v>{ Opcodes.remove_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
@@ -2384,13 +2517,13 @@
         <v>113</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="1" t="str">
+      <c r="I35" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_obj=0x8A,</v>
       </c>
       <c r="J35" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_obj=0x8A,</v>
       </c>
       <c r="K35" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2398,14 +2531,18 @@
       </c>
       <c r="L35" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M35" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M35" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N35" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print_obj, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
@@ -2424,13 +2561,13 @@
       <c r="H36" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I36" s="1" t="str">
+      <c r="I36" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ret=0x8B,</v>
       </c>
       <c r="J36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>ret=0x8B,</v>
       </c>
       <c r="K36" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2438,14 +2575,18 @@
       </c>
       <c r="L36" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M36" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M36" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N36" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.ret, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
@@ -2462,13 +2603,13 @@
         <v>119</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="1" t="str">
+      <c r="I37" s="2" t="str">
         <f t="shared" si="2"/>
         <v>jump=0x8C,</v>
       </c>
       <c r="J37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>jump=0x8C,</v>
       </c>
       <c r="K37" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2476,14 +2617,18 @@
       </c>
       <c r="L37" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M37" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M37" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N37" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.jump, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -2500,13 +2645,13 @@
         <v>122</v>
       </c>
       <c r="H38" s="2"/>
-      <c r="I38" s="1" t="str">
+      <c r="I38" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_paddr=0x8D,</v>
       </c>
       <c r="J38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_paddr=0x8D,</v>
       </c>
       <c r="K38" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2514,14 +2659,18 @@
       </c>
       <c r="L38" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M38" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M38" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N38" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print_paddr, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>5</v>
       </c>
@@ -2540,28 +2689,32 @@
         <v>125</v>
       </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="1" t="str">
+      <c r="I39" s="2" t="str">
         <f t="shared" si="2"/>
         <v>load=0x8E,</v>
       </c>
       <c r="J39" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>load=0x8E,</v>
+      </c>
+      <c r="K39" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K39" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L39" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M39" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N39" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.load, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
@@ -2580,13 +2733,13 @@
       <c r="H40" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I40" s="1" t="str">
+      <c r="I40" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rtrue=0xB0,</v>
       </c>
       <c r="J40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>rtrue=0xB0,</v>
       </c>
       <c r="K40" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2594,14 +2747,18 @@
       </c>
       <c r="L40" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M40" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M40" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N40" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.rtrue, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
@@ -2620,13 +2777,13 @@
       <c r="H41" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I41" s="1" t="str">
+      <c r="I41" s="2" t="str">
         <f t="shared" si="2"/>
         <v>rfalse=0xB1,</v>
       </c>
       <c r="J41" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>rfalse=0xB1,</v>
       </c>
       <c r="K41" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2634,14 +2791,18 @@
       </c>
       <c r="L41" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M41" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M41" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N41" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.rfalse, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
@@ -2658,13 +2819,13 @@
         <v>132</v>
       </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="1" t="str">
+      <c r="I42" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print=0xB2,</v>
       </c>
       <c r="J42" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print=0xB2,</v>
       </c>
       <c r="K42" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2672,14 +2833,18 @@
       </c>
       <c r="L42" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M42" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M42" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N42" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
@@ -2698,13 +2863,13 @@
       <c r="H43" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I43" s="1" t="str">
+      <c r="I43" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_ret=0xB3,</v>
       </c>
       <c r="J43" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_ret=0xB3,</v>
       </c>
       <c r="K43" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2712,14 +2877,18 @@
       </c>
       <c r="L43" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M43" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M43" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N43" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print_ret, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2740,28 +2909,32 @@
         <v>138</v>
       </c>
       <c r="H44" s="2"/>
-      <c r="I44" s="1" t="str">
+      <c r="I44" s="2" t="str">
         <f t="shared" si="2"/>
         <v>save=0xB5,</v>
       </c>
       <c r="J44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>save=0xB5,</v>
       </c>
       <c r="K44" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L44" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L44" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M44" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N44" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.save, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2782,28 +2955,32 @@
         <v>141</v>
       </c>
       <c r="H45" s="2"/>
-      <c r="I45" s="1" t="str">
+      <c r="I45" s="2" t="str">
         <f t="shared" si="2"/>
         <v>restore=0xB6,</v>
       </c>
       <c r="J45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>restore=0xB6,</v>
       </c>
       <c r="K45" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L45" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L45" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M45" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N45" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.restore, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
@@ -2820,13 +2997,13 @@
         <v>143</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="I46" s="1" t="str">
+      <c r="I46" s="2" t="str">
         <f t="shared" si="2"/>
         <v>restart=0xB7,</v>
       </c>
       <c r="J46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>restart=0xB7,</v>
       </c>
       <c r="K46" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2834,14 +3011,18 @@
       </c>
       <c r="L46" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M46" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M46" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N46" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.restart, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
@@ -2860,13 +3041,13 @@
       <c r="H47" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I47" s="1" t="str">
+      <c r="I47" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ret_popped=0xB8,</v>
       </c>
       <c r="J47" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>ret_popped=0xB8,</v>
       </c>
       <c r="K47" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2874,14 +3055,18 @@
       </c>
       <c r="L47" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M47" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M47" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N47" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.ret_popped, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
@@ -2900,13 +3085,13 @@
         <v>147</v>
       </c>
       <c r="H48" s="2"/>
-      <c r="I48" s="1" t="str">
+      <c r="I48" s="2" t="str">
         <f t="shared" si="2"/>
         <v>pop=0xB9,</v>
       </c>
       <c r="J48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>pop=0xB9,</v>
       </c>
       <c r="K48" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2914,14 +3099,18 @@
       </c>
       <c r="L48" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M48" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M48" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N48" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.pop, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
@@ -2940,13 +3129,13 @@
       <c r="H49" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I49" s="1" t="str">
+      <c r="I49" s="2" t="str">
         <f t="shared" si="2"/>
         <v>quit=0xBA,</v>
       </c>
       <c r="J49" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>quit=0xBA,</v>
       </c>
       <c r="K49" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2954,14 +3143,18 @@
       </c>
       <c r="L49" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M49" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M49" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N49" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.quit, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
@@ -2978,13 +3171,13 @@
         <v>151</v>
       </c>
       <c r="H50" s="2"/>
-      <c r="I50" s="1" t="str">
+      <c r="I50" s="2" t="str">
         <f t="shared" si="2"/>
         <v>new_line=0xBB,</v>
       </c>
       <c r="J50" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>new_line=0xBB,</v>
       </c>
       <c r="K50" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2992,14 +3185,18 @@
       </c>
       <c r="L50" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M50" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M50" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N50" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.new_line, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
@@ -3018,13 +3215,13 @@
         <v>153</v>
       </c>
       <c r="H51" s="2"/>
-      <c r="I51" s="1" t="str">
+      <c r="I51" s="2" t="str">
         <f t="shared" si="2"/>
         <v>show_status=0xBC,</v>
       </c>
       <c r="J51" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>show_status=0xBC,</v>
       </c>
       <c r="K51" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3032,14 +3229,18 @@
       </c>
       <c r="L51" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M51" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M51" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N51" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.show_status, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -3060,28 +3261,32 @@
         <v>156</v>
       </c>
       <c r="H52" s="2"/>
-      <c r="I52" s="1" t="str">
+      <c r="I52" s="2" t="str">
         <f t="shared" si="2"/>
         <v>verify=0xBD,</v>
       </c>
       <c r="J52" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>verify=0xBD,</v>
       </c>
       <c r="K52" s="1" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="L52" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Branch</v>
       </c>
-      <c r="L52" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="M52" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N52" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.verify, InstructionSpecialTypes.Branch},</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>5</v>
       </c>
@@ -3102,28 +3307,32 @@
         <v>159</v>
       </c>
       <c r="H53" s="2"/>
-      <c r="I53" s="1" t="str">
+      <c r="I53" s="2" t="str">
         <f t="shared" si="2"/>
         <v>call=0xE0,</v>
       </c>
       <c r="J53" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>call=0xE0,</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K53" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L53" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M53" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N53" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.call, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
@@ -3140,13 +3349,13 @@
         <v>162</v>
       </c>
       <c r="H54" s="2"/>
-      <c r="I54" s="1" t="str">
+      <c r="I54" s="2" t="str">
         <f t="shared" si="2"/>
         <v>storew=0xE1,</v>
       </c>
       <c r="J54" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>storew=0xE1,</v>
       </c>
       <c r="K54" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3154,14 +3363,18 @@
       </c>
       <c r="L54" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M54" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M54" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N54" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.storew, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
@@ -3178,13 +3391,13 @@
         <v>165</v>
       </c>
       <c r="H55" s="2"/>
-      <c r="I55" s="1" t="str">
+      <c r="I55" s="2" t="str">
         <f t="shared" si="2"/>
         <v>storeb=0xE2,</v>
       </c>
       <c r="J55" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>storeb=0xE2,</v>
       </c>
       <c r="K55" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3192,14 +3405,18 @@
       </c>
       <c r="L55" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M55" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M55" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N55" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.storeb, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
@@ -3216,13 +3433,13 @@
         <v>168</v>
       </c>
       <c r="H56" s="2"/>
-      <c r="I56" s="1" t="str">
+      <c r="I56" s="2" t="str">
         <f t="shared" si="2"/>
         <v>put_prop=0xE3,</v>
       </c>
       <c r="J56" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>put_prop=0xE3,</v>
       </c>
       <c r="K56" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3230,14 +3447,18 @@
       </c>
       <c r="L56" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M56" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M56" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N56" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.put_prop, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
@@ -3256,13 +3477,13 @@
         <v>171</v>
       </c>
       <c r="H57" s="2"/>
-      <c r="I57" s="1" t="str">
+      <c r="I57" s="2" t="str">
         <f t="shared" si="2"/>
         <v>sread=0xE4,</v>
       </c>
       <c r="J57" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>sread=0xE4,</v>
       </c>
       <c r="K57" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3270,14 +3491,18 @@
       </c>
       <c r="L57" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M57" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M57" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N57" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.sread, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
@@ -3294,13 +3519,13 @@
         <v>174</v>
       </c>
       <c r="H58" s="2"/>
-      <c r="I58" s="1" t="str">
+      <c r="I58" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_char=0xE5,</v>
       </c>
       <c r="J58" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_char=0xE5,</v>
       </c>
       <c r="K58" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3308,14 +3533,18 @@
       </c>
       <c r="L58" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M58" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M58" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N58" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print_char, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
@@ -3332,13 +3561,13 @@
         <v>177</v>
       </c>
       <c r="H59" s="2"/>
-      <c r="I59" s="1" t="str">
+      <c r="I59" s="2" t="str">
         <f t="shared" si="2"/>
         <v>print_num=0xE6,</v>
       </c>
       <c r="J59" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>print_num=0xE6,</v>
       </c>
       <c r="K59" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3346,14 +3575,18 @@
       </c>
       <c r="L59" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M59" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M59" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N59" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.print_num, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
@@ -3372,28 +3605,32 @@
         <v>180</v>
       </c>
       <c r="H60" s="2"/>
-      <c r="I60" s="1" t="str">
+      <c r="I60" s="2" t="str">
         <f t="shared" si="2"/>
         <v>random=0xE7,</v>
       </c>
       <c r="J60" s="1" t="str">
         <f t="shared" si="3"/>
+        <v>random=0xE7,</v>
+      </c>
+      <c r="K60" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Store</v>
       </c>
-      <c r="K60" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L60" s="1" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M60" s="1" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N60" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.random, InstructionSpecialTypes.Store},</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
@@ -3410,13 +3647,13 @@
         <v>183</v>
       </c>
       <c r="H61" s="2"/>
-      <c r="I61" s="1" t="str">
+      <c r="I61" s="2" t="str">
         <f t="shared" si="2"/>
         <v>push=0xE8,</v>
       </c>
       <c r="J61" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>push=0xE8,</v>
       </c>
       <c r="K61" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3424,14 +3661,18 @@
       </c>
       <c r="L61" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M61" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M61" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N61" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.push, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
@@ -3450,13 +3691,13 @@
         <v>186</v>
       </c>
       <c r="H62" s="2"/>
-      <c r="I62" s="1" t="str">
+      <c r="I62" s="2" t="str">
         <f t="shared" si="2"/>
         <v>pull=0xE9,</v>
       </c>
       <c r="J62" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>pull=0xE9,</v>
       </c>
       <c r="K62" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3464,14 +3705,18 @@
       </c>
       <c r="L62" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M62" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M62" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N62" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.pull, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
@@ -3490,13 +3735,13 @@
         <v>189</v>
       </c>
       <c r="H63" s="2"/>
-      <c r="I63" s="1" t="str">
+      <c r="I63" s="2" t="str">
         <f t="shared" si="2"/>
         <v>split_window=0xEA,</v>
       </c>
       <c r="J63" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>split_window=0xEA,</v>
       </c>
       <c r="K63" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3504,14 +3749,18 @@
       </c>
       <c r="L63" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M63" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M63" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N63" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.split_window, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
@@ -3530,13 +3779,13 @@
         <v>192</v>
       </c>
       <c r="H64" s="2"/>
-      <c r="I64" s="1" t="str">
+      <c r="I64" s="2" t="str">
         <f t="shared" si="2"/>
         <v>set_window=0xEB,</v>
       </c>
       <c r="J64" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>set_window=0xEB,</v>
       </c>
       <c r="K64" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3544,14 +3793,18 @@
       </c>
       <c r="L64" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M64" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M64" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N64" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.set_window, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
@@ -3570,13 +3823,13 @@
         <v>195</v>
       </c>
       <c r="H65" s="2"/>
-      <c r="I65" s="1" t="str">
+      <c r="I65" s="2" t="str">
         <f t="shared" si="2"/>
         <v>output_stream=0xF3,</v>
       </c>
       <c r="J65" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>output_stream=0xF3,</v>
       </c>
       <c r="K65" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3584,14 +3837,18 @@
       </c>
       <c r="L65" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M65" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M65" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="N65" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>{ Opcodes.output_stream, InstructionSpecialTypes.None},</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
@@ -3610,13 +3867,13 @@
         <v>198</v>
       </c>
       <c r="H66" s="2"/>
-      <c r="I66" s="1" t="str">
+      <c r="I66" s="2" t="str">
         <f t="shared" si="2"/>
         <v>input_stream=0xF4,</v>
       </c>
       <c r="J66" s="1" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>input_stream=0xF4,</v>
       </c>
       <c r="K66" s="1" t="str">
         <f t="shared" si="4"/>
@@ -3624,10 +3881,14 @@
       </c>
       <c r="L66" s="1" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M66" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>None</v>
       </c>
-      <c r="M66" s="1" t="str">
-        <f t="shared" ref="M66:M97" si="7">"{ Opcodes." &amp; G66 &amp; ", InstructionSpecialTypes." &amp; J66 &amp; K66 &amp; L66 &amp; "},"</f>
+      <c r="N66" s="1" t="str">
+        <f t="shared" ref="N66" si="8">"{ Opcodes." &amp; G66 &amp; ", InstructionSpecialTypes." &amp; K66 &amp; L66 &amp; M66 &amp; "},"</f>
         <v>{ Opcodes.input_stream, InstructionSpecialTypes.None},</v>
       </c>
     </row>

</xml_diff>